<commit_message>
Updated xlsx with correct color coding and tokens
</commit_message>
<xml_diff>
--- a/assets/apim retry policy update july 3 2023.xlsx
+++ b/assets/apim retry policy update july 3 2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\azure-openai-api-m-retry\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E964D4C-0933-467F-B594-FD9297A8DFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF8DBC0-0D37-479F-AE52-600850A89912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{FB2C0EC4-7131-4630-A838-D623D2BEB14F}"/>
   </bookViews>
@@ -343,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -374,8 +374,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,7 +725,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.7265625" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
@@ -875,42 +873,44 @@
         <v>5</v>
       </c>
       <c r="H5" s="8">
-        <v>240000</v>
+        <v>40000</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="1"/>
-        <v>7200</v>
+        <v>1200</v>
       </c>
       <c r="J5" s="7">
         <f t="shared" si="2"/>
-        <v>120</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1">
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="8">
         <v>200000</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="7">
         <f t="shared" ref="I6" si="3">G6*((H6/1000)*6)</f>
         <v>3600</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="7">
         <f t="shared" ref="J6" si="4">I6/60</f>
         <v>60</v>
       </c>

</xml_diff>